<commit_message>
Lex complete minus acceptance of double operators ie. ++, --, &&, and ||
</commit_message>
<xml_diff>
--- a/CompilerProject/Resources/table.xlsx
+++ b/CompilerProject/Resources/table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sales\source\repos\CompilerProject\CompilerProject\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B79F4EB-70D3-4197-A5B1-4F7E3245D8B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90F426C-DA37-49D0-9E67-0AF3951E3C00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{52CB5B26-32AE-45D7-A2C6-F659E41807B2}"/>
   </bookViews>
@@ -488,7 +488,7 @@
   <dimension ref="A1:AH14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="AH15" sqref="AH15"/>
+      <selection activeCell="AE3" sqref="AE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,11 +606,11 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
       <c r="W3">
         <v>3</v>
+      </c>
+      <c r="AE3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added instructions to code generator
</commit_message>
<xml_diff>
--- a/CompilerProject/Resources/table.xlsx
+++ b/CompilerProject/Resources/table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sales\source\repos\CompilerProject\CompilerProject\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90F426C-DA37-49D0-9E67-0AF3951E3C00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6697B7F7-3CC9-41EB-B396-D3EB2455C79D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{52CB5B26-32AE-45D7-A2C6-F659E41807B2}"/>
   </bookViews>
@@ -488,7 +488,7 @@
   <dimension ref="A1:AH14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,9 +606,6 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="W3">
-        <v>3</v>
-      </c>
       <c r="AE3">
         <v>2</v>
       </c>
@@ -617,6 +614,9 @@
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="W4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -683,6 +683,9 @@
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
+      </c>
+      <c r="M9">
+        <v>4</v>
       </c>
       <c r="N9">
         <v>3</v>

</xml_diff>